<commit_message>
Update CNN, Cables Repartition & Gantt Diagram
</commit_message>
<xml_diff>
--- a/CableRepartition.xlsx
+++ b/CableRepartition.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gaizi\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\evaux\Documents\Internship_Projects\4_Robot\Robot_Project_IFX\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14100"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12432"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="61">
   <si>
     <t xml:space="preserve">Cables </t>
   </si>
@@ -56,12 +56,6 @@
     <t>Left Encoder VCC</t>
   </si>
   <si>
-    <t>VCC Battery Power Supply</t>
-  </si>
-  <si>
-    <t>Ground of Battery Power supply</t>
-  </si>
-  <si>
     <t>Right Encoder VCC</t>
   </si>
   <si>
@@ -77,12 +71,6 @@
     <t>H-Bridge to Left Motor (Blue Cable)</t>
   </si>
   <si>
-    <t>52 - 5</t>
-  </si>
-  <si>
-    <t>58 - 6</t>
-  </si>
-  <si>
     <t>60 - 25</t>
   </si>
   <si>
@@ -129,6 +117,96 @@
   </si>
   <si>
     <t>OUT4 H-Bridge</t>
+  </si>
+  <si>
+    <t>Alim_Aurix</t>
+  </si>
+  <si>
+    <t>GND</t>
+  </si>
+  <si>
+    <t>AN1</t>
+  </si>
+  <si>
+    <t>5V</t>
+  </si>
+  <si>
+    <t>Pin up to the AO of the 1st current sensor &lt;-&gt; 60 - 24</t>
+  </si>
+  <si>
+    <t>One of the 2 pins near the Capacitor of the 1st current sensor &lt;-&gt; 55 - 10</t>
+  </si>
+  <si>
+    <t>57- 6</t>
+  </si>
+  <si>
+    <t>Ground of Battery Power supply (8V)</t>
+  </si>
+  <si>
+    <t>Ground of Battery Power supply (5V)</t>
+  </si>
+  <si>
+    <t>VCC Battery Power Supply (8V)</t>
+  </si>
+  <si>
+    <t>VCC Battery Power Supply (5V)</t>
+  </si>
+  <si>
+    <t>Red mark on the 1st current sensor</t>
+  </si>
+  <si>
+    <t>Blue mark on the 1st current sensor &lt;-&gt; 50 - 5</t>
+  </si>
+  <si>
+    <t>Black mark on the 1st current sensor &lt;-&gt; 57 - 6</t>
+  </si>
+  <si>
+    <t>Alim_servo</t>
+  </si>
+  <si>
+    <t>Blue mark on the 2nd current sensor &lt;-&gt; 55-1</t>
+  </si>
+  <si>
+    <t>Alim_Rasp</t>
+  </si>
+  <si>
+    <t>Black mark on the 2nd current sensor &lt;-&gt; Power bank</t>
+  </si>
+  <si>
+    <t>Red mark on the 2nd current sensor &lt;-&gt; Power bank</t>
+  </si>
+  <si>
+    <t>Blue mark on the 2nd current sensor &lt;-&gt; Raspberry</t>
+  </si>
+  <si>
+    <t>Black mark on the first current sensor &lt;-&gt; Raspberry</t>
+  </si>
+  <si>
+    <t>Black mark on the first current sensor &lt;-&gt; 57 - 24</t>
+  </si>
+  <si>
+    <t>Pin up to the AO of the 2nd current sensor &lt;-&gt; 60 - 23</t>
+  </si>
+  <si>
+    <t>AN2</t>
+  </si>
+  <si>
+    <t>One of the 2 pins near the Capacitor of the 2nd current sensor &lt;-&gt; 55 - 9</t>
+  </si>
+  <si>
+    <t>RX_aurix</t>
+  </si>
+  <si>
+    <t>TX_aurix</t>
+  </si>
+  <si>
+    <t>58 - 36 &lt;-&gt; W label of the Raspberry</t>
+  </si>
+  <si>
+    <t>57 - 36 &lt;-&gt; B label of the Raspberry</t>
+  </si>
+  <si>
+    <t>56 - 36 &lt;-&gt; G label of the Raspberry</t>
   </si>
 </sst>
 </file>
@@ -221,7 +299,7 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="2"/>
@@ -229,6 +307,7 @@
     <xf numFmtId="17" fontId="1" fillId="4" borderId="0" xfId="3" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="4"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="3" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="2" applyFont="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="40% - Accent2" xfId="2" builtinId="35"/>
@@ -513,20 +592,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:C32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="35.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.5703125" customWidth="1"/>
-    <col min="3" max="3" width="30.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="35.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5546875" customWidth="1"/>
+    <col min="3" max="3" width="60.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -534,32 +613,32 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>11</v>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="7" t="s">
+        <v>38</v>
       </c>
       <c r="B2" s="5">
         <v>1</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>10</v>
+      <c r="C2" s="6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="7" t="s">
+        <v>40</v>
       </c>
       <c r="B3" s="5">
         <v>2</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C3" s="6" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>9</v>
       </c>
@@ -567,10 +646,10 @@
         <v>3</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>2</v>
       </c>
@@ -578,10 +657,10 @@
         <v>4</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>3</v>
       </c>
@@ -589,10 +668,10 @@
         <v>5</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>4</v>
       </c>
@@ -600,10 +679,10 @@
         <v>6</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>5</v>
       </c>
@@ -611,10 +690,10 @@
         <v>7</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>6</v>
       </c>
@@ -622,10 +701,10 @@
         <v>8</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>7</v>
       </c>
@@ -633,10 +712,10 @@
         <v>9</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>8</v>
       </c>
@@ -644,79 +723,241 @@
         <v>10</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B12" s="5">
         <v>11</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B13" s="5">
         <v>12</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B14" s="5">
         <v>13</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B15" s="5">
         <v>14</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B16" s="5">
         <v>15</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B17" s="5">
         <v>16</v>
       </c>
       <c r="C17" s="6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B18" s="5">
+        <v>17</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B19" s="5">
+        <v>18</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" s="7" t="s">
         <v>34</v>
+      </c>
+      <c r="B20" s="5">
+        <v>19</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B21" s="5">
+        <v>20</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="B22" s="5">
+        <v>21</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="B23" s="5">
+        <v>22</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="B24" s="5">
+        <v>23</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B25" s="5">
+        <v>24</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B26" s="5">
+        <v>25</v>
+      </c>
+      <c r="C26" s="6" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B27" s="5">
+        <v>26</v>
+      </c>
+      <c r="C27" s="6" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B28" s="5">
+        <v>27</v>
+      </c>
+      <c r="C28" s="6" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A29" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="B29" s="5">
+        <v>28</v>
+      </c>
+      <c r="C29" s="6" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A30" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B30" s="5">
+        <v>29</v>
+      </c>
+      <c r="C30" s="6" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A31" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="B31" s="5">
+        <v>30</v>
+      </c>
+      <c r="C31" s="6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A32" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="B32" s="5">
+        <v>31</v>
+      </c>
+      <c r="C32" s="6" t="s">
+        <v>60</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <ignoredErrors>
-    <ignoredError sqref="C12:C13" twoDigitTextYear="1"/>
-  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>